<commit_message>
commiting the complete project code including the excel file
</commit_message>
<xml_diff>
--- a/src/test/resources/acti/testdata/actidata.xlsx
+++ b/src/test/resources/acti/testdata/actidata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WORKSPACE\BATCH20\com.qa.actitime\src\test\resources\acti\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shahr\git\actitime.automation\src\test\resources\acti\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33A0030D-A9EF-4EFA-9047-5D5DACFBFAC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A0A2033-1961-4248-BD77-BB80CB32A6FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1750" yWindow="1140" windowWidth="14400" windowHeight="7350" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -351,7 +351,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>